<commit_message>
Extent Report Configuration is done
</commit_message>
<xml_diff>
--- a/src/test/java/soFi/TMDB/Api/InputData/Authentication_TestData.xlsx
+++ b/src/test/java/soFi/TMDB/Api/InputData/Authentication_TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E85ED7C-F8C4-4EF2-B09C-8AED0108C590}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F2E6A6-3844-4946-A038-BE5D6BAA9DA3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18990" windowHeight="12870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
   <si>
     <t>1</t>
   </si>
@@ -46,18 +46,6 @@
     <t>200</t>
   </si>
   <si>
-    <t>ExpectedHttpCode</t>
-  </si>
-  <si>
-    <t>Expectedstatus_message</t>
-  </si>
-  <si>
-    <t>Expectedsuccess</t>
-  </si>
-  <si>
-    <t>Expectedstatus_code</t>
-  </si>
-  <si>
     <t>Test Response for Invalid Response</t>
   </si>
   <si>
@@ -115,22 +103,40 @@
     <t>TS01_TC02_Authencation_CreateTestToken_Get_With_invalid_Key</t>
   </si>
   <si>
-    <t>TS01_TC02_Authencation_CreateTestToken_Get_With_Invalid_Resource</t>
-  </si>
-  <si>
-    <t>TS01_TC03_Authencation_CreateTestToken_Get_With_Invalid_Resource_TestData</t>
-  </si>
-  <si>
     <t>TS01_TC02_Authencation_CreateTestToken_Get_With_invalid_Key_TestData</t>
   </si>
   <si>
-    <t>ExpectedgetStatusCode</t>
-  </si>
-  <si>
     <t>Invalid_api_key</t>
   </si>
   <si>
     <t>b0c049db340cadd406e370aea287fabc</t>
+  </si>
+  <si>
+    <t>status_message</t>
+  </si>
+  <si>
+    <t>success</t>
+  </si>
+  <si>
+    <t>status_code</t>
+  </si>
+  <si>
+    <t>getStatusCode</t>
+  </si>
+  <si>
+    <t>TS01_TC03_Authencation_CreateTestToken_Get_With_invalid_Resource_TestData</t>
+  </si>
+  <si>
+    <t>TS01_TC03_Authencation_CreateTestToken_Get_With_Invalid_Resource</t>
+  </si>
+  <si>
+    <t>The resource you requested could not be found.</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>Validate Expected Response with  InValid Resource Request</t>
   </si>
 </sst>
 </file>
@@ -545,7 +551,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,16 +561,14 @@
     <col min="3" max="3" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="44.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -581,24 +585,24 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>6</v>
@@ -611,7 +615,7 @@
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H3" s="3"/>
     </row>
@@ -634,7 +638,7 @@
     </row>
     <row r="6" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -651,27 +655,27 @@
         <v>1</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>6</v>
@@ -680,19 +684,19 @@
         <v>0</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="I8" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -711,7 +715,7 @@
     </row>
     <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -727,26 +731,22 @@
       <c r="D12" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="F12" s="4" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>6</v>
@@ -754,18 +754,14 @@
       <c r="D13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="6"/>
+      <c r="E13" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="F13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>25</v>
+        <v>36</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -792,10 +788,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -808,26 +804,25 @@
       <c r="D17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="F17" s="4" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="H17" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>6</v>
@@ -835,20 +830,19 @@
       <c r="D18" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>6</v>
@@ -856,34 +850,32 @@
       <c r="D19" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="E19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Final Clean Version of the Project Ready for Continuous Integration.
</commit_message>
<xml_diff>
--- a/src/test/java/soFi/TMDB/Api/InputData/Authentication_TestData.xlsx
+++ b/src/test/java/soFi/TMDB/Api/InputData/Authentication_TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F2E6A6-3844-4946-A038-BE5D6BAA9DA3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2D6D6B-BA4B-46EF-94AA-D1DE8C09597C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18990" windowHeight="12870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="40">
   <si>
     <t>1</t>
   </si>
@@ -28,9 +28,6 @@
     <t>RowID</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>TestCaseDescription</t>
   </si>
   <si>
@@ -46,30 +43,6 @@
     <t>200</t>
   </si>
   <si>
-    <t>Test Response for Invalid Response</t>
-  </si>
-  <si>
-    <t>Test Response for InValid API Key</t>
-  </si>
-  <si>
-    <t>Test Response for Valid API Key</t>
-  </si>
-  <si>
-    <t>Authencation_CreateSession_Get_TestData</t>
-  </si>
-  <si>
-    <t>TS01_TC04_Authencation_CreateSession_Get</t>
-  </si>
-  <si>
-    <t>TS01_TC05_Authencation_CreateSession_Get</t>
-  </si>
-  <si>
-    <t>TS01_TC06_Authencation_CreateSession_Get</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>401</t>
   </si>
   <si>
@@ -88,12 +61,6 @@
     <t>7</t>
   </si>
   <si>
-    <t>Validate Expected Response with  InValid API Key Request</t>
-  </si>
-  <si>
-    <t>Validate Expected Response with  Valid API Key Request</t>
-  </si>
-  <si>
     <t>TS01_TC01_Authencation_CreateTestToken_Get_With_Valid_Key</t>
   </si>
   <si>
@@ -136,7 +103,43 @@
     <t>34</t>
   </si>
   <si>
-    <t>Validate Expected Response with  InValid Resource Request</t>
+    <t>TS01_TC04_Authencation_Create_Session_Get_With_Valid_Api_key_TestData</t>
+  </si>
+  <si>
+    <t>TS01_TC04_Authencation_Create_Session_Get_With_Valid_Api_key</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>arpans2112</t>
+  </si>
+  <si>
+    <t>@rpaN@2648169</t>
+  </si>
+  <si>
+    <t>TS1_TC05_Authentication_CreateSessionWithLogin_Get_With_Valid_Key</t>
+  </si>
+  <si>
+    <t>TS1_TC05_Authentication_CreateSessionWithLogin_Get_With_Valid_Key_TestData</t>
+  </si>
+  <si>
+    <t>Validate Expected Response of [Create Test Token ] Get Method, with  InValid Resource Request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate Expected Response of [Creation Session] Get Method, with Valid API Key </t>
+  </si>
+  <si>
+    <t>Validate Response of [Create Session with Login] Get Method, with Valid API Key</t>
+  </si>
+  <si>
+    <t>Validate Expected Response of [Create Test Token] Get Method, with  InValid API Key Request</t>
+  </si>
+  <si>
+    <t>Validate Expected Response of [Create Test Token] Get Method, with  Valid API Key Request</t>
   </si>
 </sst>
 </file>
@@ -212,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -234,6 +237,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,80 +563,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="75.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="75.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" style="13" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="44.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
@@ -631,83 +647,83 @@
       <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="9"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="10"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>38</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="10"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="I9" s="11"/>
     </row>
     <row r="10" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="10"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
@@ -715,58 +731,58 @@
     </row>
     <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="C13" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="10"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
@@ -777,7 +793,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="10"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
@@ -788,94 +804,139 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>10</v>
+        <v>28</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>36</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="2" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="J23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>